<commit_message>
add balanced binary tree
</commit_message>
<xml_diff>
--- a/leet_questions.xlsx
+++ b/leet_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/Documents/PycharmProjects/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55AC708-3003-1F4F-BB82-684339F79D55}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48CB93A-52FB-C64A-A7B6-A85B62DDBB8B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56060" yWindow="500" windowWidth="29020" windowHeight="21100" xr2:uid="{6494FC7B-E176-1246-80FA-A19190C52CC5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="61">
   <si>
     <t>No.</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>diameter of binary tree</t>
+  </si>
+  <si>
+    <t>balanced binary tree</t>
   </si>
 </sst>
 </file>
@@ -601,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0133E33A-35EB-C641-A01A-836B9FBF889B}">
-  <dimension ref="A1:P23"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1314,6 +1317,38 @@
         <v>22</v>
       </c>
     </row>
+    <row r="24" spans="1:13" ht="17">
+      <c r="A24" s="1">
+        <v>110</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45200</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1">
+        <v>7</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add [linkedlist] remove duplicate
</commit_message>
<xml_diff>
--- a/leet_questions.xlsx
+++ b/leet_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kai/Documents/PycharmProjects/interview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA918108-215A-944D-938F-EE6A8803D303}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E887BB-54BB-2D4F-A6CB-19389FCEE626}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="860" windowWidth="32100" windowHeight="21100" xr2:uid="{6494FC7B-E176-1246-80FA-A19190C52CC5}"/>
+    <workbookView xWindow="2460" yWindow="860" windowWidth="32100" windowHeight="21100" activeTab="1" xr2:uid="{6494FC7B-E176-1246-80FA-A19190C52CC5}"/>
   </bookViews>
   <sheets>
     <sheet name="leetcode" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="82">
   <si>
     <t>No.</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>dynamic programming</t>
+  </si>
+  <si>
+    <t>remove duplicate</t>
+  </si>
+  <si>
+    <t>linkedlist</t>
   </si>
 </sst>
 </file>
@@ -665,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0133E33A-35EB-C641-A01A-836B9FBF889B}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
@@ -1635,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189899C0-1422-2A42-A391-202CE1972FFE}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1834,17 +1840,37 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+    <row r="6" spans="1:16" ht="34">
+      <c r="A6" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6">
+        <v>45221</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>

</xml_diff>